<commit_message>
consolidated data into a single satellite, added google translate, fixed tooltip
</commit_message>
<xml_diff>
--- a/satellites_combined_sealevel_year.xlsx
+++ b/satellites_combined_sealevel_year.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="134" documentId="8_{162EEE67-341B-4313-8EBB-193D051E45A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33E549B8-E553-405C-AAB5-7B83B881636D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{578984C9-7CA1-4DD9-859D-8DCFE58795FE}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12180" windowHeight="15370" xr2:uid="{578984C9-7CA1-4DD9-859D-8DCFE58795FE}"/>
   </bookViews>
   <sheets>
     <sheet name="slr_sla_gbl_keep_all_66" sheetId="1" r:id="rId1"/>
@@ -590,6 +590,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -909,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722A5E30-6EF6-4534-A4D8-85641C255695}">
   <dimension ref="A1:C1539"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A1079" zoomScale="62" workbookViewId="0">
+      <selection activeCell="B1096" sqref="B1096:B1100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>